<commit_message>
Project 1 Finished Datapath
</commit_message>
<xml_diff>
--- a/cs2200-project1/microcode/microcode.xlsx
+++ b/cs2200-project1/microcode/microcode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nandhasundaravadivel/Documents/2200/cs2200-project1/microcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF3422AF-8113-F246-9E63-2182B79FC243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89A0A78-0D10-0E45-9A49-9286949E21ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30200" yWindow="-1020" windowWidth="27620" windowHeight="14920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51200" yWindow="-14400" windowWidth="25380" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="74">
   <si>
     <t>Index</t>
   </si>
@@ -271,6 +271,42 @@
   </si>
   <si>
     <t>Fetch3</t>
+  </si>
+  <si>
+    <t>ADD1</t>
+  </si>
+  <si>
+    <t>ADD2</t>
+  </si>
+  <si>
+    <t>ADD3</t>
+  </si>
+  <si>
+    <t>NAND1</t>
+  </si>
+  <si>
+    <t>NAND2</t>
+  </si>
+  <si>
+    <t>NAND3</t>
+  </si>
+  <si>
+    <t>ADDI1</t>
+  </si>
+  <si>
+    <t>ADDI2</t>
+  </si>
+  <si>
+    <t>ADDI3</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>ADD $t0, T1, $t2</t>
+  </si>
+  <si>
+    <t>00000110011100000000000000001000'</t>
   </si>
 </sst>
 </file>
@@ -519,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -581,6 +617,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -633,6 +670,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,9 +901,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y56" sqref="Y56"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE4" sqref="AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -896,14 +934,14 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
       <c r="I1" s="9" t="s">
         <v>3</v>
       </c>
@@ -1264,9 +1302,9 @@
         <v>0</v>
       </c>
       <c r="AD4" s="2"/>
-      <c r="AE4" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>0E00900</v>
+      <c r="AE4" s="23" t="e">
+        <f>_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(AC4,AB4),1),BIN2HEX(_xlfn.CONCAT(AA4,4,Y4,X4),1),BIN2HEX(_xlfn.CONCAT(W4,V4,U4,T4),1),BIN2HEX(_xlfn.CONCAT(S4,R4,Q4,P4),1),BIN2HEX(_xlfn.CONCAT(O4,N4,M4,L4),1),BIN2HEX(_xlfn.CONCAT(K4,J4,C4,D4),1),BIN2HEX(_xlfn.CONCAT(E4,F4,G4,H4),1))</f>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="5" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1368,7 +1406,9 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="C6" s="4">
         <v>0</v>
       </c>
@@ -1379,20 +1419,20 @@
         <v>0</v>
       </c>
       <c r="F6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
       </c>
       <c r="H6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="4">
         <v>0</v>
@@ -1416,7 +1456,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" s="4">
         <v>0</v>
@@ -1454,7 +1494,7 @@
       <c r="AD6" s="2"/>
       <c r="AE6" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>0004045</v>
       </c>
     </row>
     <row r="7" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1462,7 +1502,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>63</v>
+      </c>
       <c r="C7" s="4">
         <v>0</v>
       </c>
@@ -1473,20 +1515,20 @@
         <v>0</v>
       </c>
       <c r="F7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="4">
         <v>0</v>
       </c>
       <c r="I7" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J7" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="4">
         <v>0</v>
@@ -1513,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="S7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7" s="4">
         <v>0</v>
@@ -1525,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="W7" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7" s="4">
         <v>0</v>
@@ -1548,7 +1590,7 @@
       <c r="AD7" s="2"/>
       <c r="AE7" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>0088046</v>
       </c>
     </row>
     <row r="8" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1556,7 +1598,9 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="C8" s="4">
         <v>0</v>
       </c>
@@ -1586,7 +1630,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="12">
         <v>0</v>
@@ -1613,7 +1657,7 @@
         <v>0</v>
       </c>
       <c r="U8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" s="4">
         <v>0</v>
@@ -1622,7 +1666,7 @@
         <v>0</v>
       </c>
       <c r="X8" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="4">
         <v>0</v>
@@ -1642,7 +1686,7 @@
       <c r="AD8" s="2"/>
       <c r="AE8" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>0120100</v>
       </c>
     </row>
     <row r="9" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1744,7 +1788,9 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="C10" s="4">
         <v>0</v>
       </c>
@@ -1752,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="4">
         <v>0</v>
@@ -1761,14 +1807,14 @@
         <v>0</v>
       </c>
       <c r="H10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J10" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="4">
         <v>0</v>
@@ -1792,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="R10" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10" s="4">
         <v>0</v>
@@ -1813,7 +1859,7 @@
         <v>0</v>
       </c>
       <c r="Y10" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10" s="4">
         <v>0</v>
@@ -1830,7 +1876,7 @@
       <c r="AD10" s="2"/>
       <c r="AE10" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>0204049</v>
       </c>
     </row>
     <row r="11" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1838,7 +1884,9 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="C11" s="4">
         <v>0</v>
       </c>
@@ -1846,23 +1894,23 @@
         <v>0</v>
       </c>
       <c r="E11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
       </c>
       <c r="G11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="4">
         <v>0</v>
       </c>
       <c r="I11" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J11" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="4">
         <v>0</v>
@@ -1889,7 +1937,7 @@
         <v>0</v>
       </c>
       <c r="S11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11" s="4">
         <v>0</v>
@@ -1901,13 +1949,13 @@
         <v>0</v>
       </c>
       <c r="W11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11" s="4">
         <v>0</v>
       </c>
       <c r="Y11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11" s="4">
         <v>0</v>
@@ -1924,7 +1972,7 @@
       <c r="AD11" s="2"/>
       <c r="AE11" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>028804A</v>
       </c>
     </row>
     <row r="12" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1932,7 +1980,9 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="C12" s="4">
         <v>0</v>
       </c>
@@ -1962,7 +2012,7 @@
         <v>0</v>
       </c>
       <c r="L12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="12">
         <v>0</v>
@@ -1989,7 +2039,7 @@
         <v>0</v>
       </c>
       <c r="U12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12" s="4">
         <v>0</v>
@@ -1998,10 +2048,10 @@
         <v>0</v>
       </c>
       <c r="X12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y12" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z12" s="4">
         <v>0</v>
@@ -2018,7 +2068,7 @@
       <c r="AD12" s="2"/>
       <c r="AE12" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>0320100</v>
       </c>
     </row>
     <row r="13" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2120,7 +2170,9 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="C14" s="4">
         <v>0</v>
       </c>
@@ -2128,23 +2180,23 @@
         <v>0</v>
       </c>
       <c r="E14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
       </c>
       <c r="H14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J14" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="4">
         <v>0</v>
@@ -2168,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14" s="4">
         <v>0</v>
@@ -2183,7 +2235,7 @@
         <v>0</v>
       </c>
       <c r="W14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X14" s="4">
         <v>0</v>
@@ -2206,7 +2258,7 @@
       <c r="AD14" s="2"/>
       <c r="AE14" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>008404D</v>
       </c>
     </row>
     <row r="15" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2214,7 +2266,9 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="C15" s="4">
         <v>0</v>
       </c>
@@ -2222,20 +2276,20 @@
         <v>0</v>
       </c>
       <c r="E15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="4">
         <v>0</v>
       </c>
       <c r="I15" s="11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J15" s="12">
         <v>0</v>
@@ -2250,7 +2304,7 @@
         <v>0</v>
       </c>
       <c r="N15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" s="4">
         <v>0</v>
@@ -2265,7 +2319,7 @@
         <v>0</v>
       </c>
       <c r="S15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T15" s="4">
         <v>0</v>
@@ -2300,7 +2354,7 @@
       <c r="AD15" s="2"/>
       <c r="AE15" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>000840E</v>
       </c>
     </row>
     <row r="16" spans="1:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2308,7 +2362,9 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="C16" s="4">
         <v>0</v>
       </c>
@@ -2338,7 +2394,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="12">
         <v>0</v>
@@ -2365,7 +2421,7 @@
         <v>0</v>
       </c>
       <c r="U16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V16" s="4">
         <v>0</v>
@@ -2374,7 +2430,7 @@
         <v>0</v>
       </c>
       <c r="X16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y16" s="4">
         <v>0</v>
@@ -2394,7 +2450,7 @@
       <c r="AD16" s="2"/>
       <c r="AE16" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0000000</v>
+        <v>0120100</v>
       </c>
     </row>
     <row r="17" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -5510,30 +5566,30 @@
       <c r="AD52" s="2"/>
     </row>
     <row r="53" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="39" t="s">
+      <c r="B53" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="40"/>
-      <c r="G53" s="40"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="41"/>
-      <c r="J53" s="42"/>
-      <c r="L53" s="39" t="s">
+      <c r="C53" s="41"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="42"/>
+      <c r="J53" s="43"/>
+      <c r="L53" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="M53" s="41"/>
-      <c r="N53" s="41"/>
-      <c r="O53" s="42"/>
-      <c r="Q53" s="27" t="s">
+      <c r="M53" s="42"/>
+      <c r="N53" s="42"/>
+      <c r="O53" s="43"/>
+      <c r="Q53" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="R53" s="28"/>
-      <c r="S53" s="28"/>
-      <c r="T53" s="28"/>
-      <c r="U53" s="28"/>
+      <c r="R53" s="29"/>
+      <c r="S53" s="29"/>
+      <c r="T53" s="29"/>
+      <c r="U53" s="29"/>
       <c r="V53" s="21"/>
       <c r="W53" s="21"/>
       <c r="X53" s="21"/>
@@ -5557,14 +5613,14 @@
       <c r="B54" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C54" s="43" t="s">
+      <c r="C54" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="D54" s="44"/>
-      <c r="E54" s="44"/>
-      <c r="F54" s="44"/>
-      <c r="G54" s="44"/>
-      <c r="H54" s="44"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="45"/>
       <c r="I54" s="1" t="s">
         <v>25</v>
       </c>
@@ -5583,11 +5639,11 @@
       <c r="O54" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="Q54" s="28"/>
-      <c r="R54" s="28"/>
-      <c r="S54" s="28"/>
-      <c r="T54" s="28"/>
-      <c r="U54" s="28"/>
+      <c r="Q54" s="29"/>
+      <c r="R54" s="29"/>
+      <c r="S54" s="29"/>
+      <c r="T54" s="29"/>
+      <c r="U54" s="29"/>
       <c r="V54" s="21"/>
       <c r="W54" s="21"/>
       <c r="X54" s="21"/>
@@ -5611,12 +5667,12 @@
       <c r="B55" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="45"/>
-      <c r="D55" s="46"/>
-      <c r="E55" s="46"/>
-      <c r="F55" s="46"/>
-      <c r="G55" s="46"/>
-      <c r="H55" s="46"/>
+      <c r="C55" s="46"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="47"/>
+      <c r="H55" s="47"/>
       <c r="I55" s="4"/>
       <c r="J55" s="14" t="str">
         <f>DEC2HEX(C55)</f>
@@ -5628,16 +5684,18 @@
       <c r="M55" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="N55" s="2"/>
+      <c r="N55" s="2">
+        <v>5</v>
+      </c>
       <c r="O55" s="14" t="str">
         <f t="shared" ref="O55:O70" si="3">DEC2HEX(N55,2)</f>
-        <v>00</v>
-      </c>
-      <c r="Q55" s="28"/>
-      <c r="R55" s="28"/>
-      <c r="S55" s="28"/>
-      <c r="T55" s="28"/>
-      <c r="U55" s="28"/>
+        <v>05</v>
+      </c>
+      <c r="Q55" s="29"/>
+      <c r="R55" s="29"/>
+      <c r="S55" s="29"/>
+      <c r="T55" s="29"/>
+      <c r="U55" s="29"/>
       <c r="V55" s="21"/>
       <c r="W55" s="21"/>
       <c r="X55" s="21"/>
@@ -5661,12 +5719,12 @@
       <c r="B56" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="25"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="26"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
       <c r="I56" s="15"/>
       <c r="J56" s="16" t="str">
         <f>DEC2HEX(C56)</f>
@@ -5678,16 +5736,18 @@
       <c r="M56" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="N56" s="2"/>
+      <c r="N56" s="2">
+        <v>8</v>
+      </c>
       <c r="O56" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>00</v>
-      </c>
-      <c r="Q56" s="28"/>
-      <c r="R56" s="28"/>
-      <c r="S56" s="28"/>
-      <c r="T56" s="28"/>
-      <c r="U56" s="28"/>
+        <v>08</v>
+      </c>
+      <c r="Q56" s="29"/>
+      <c r="R56" s="29"/>
+      <c r="S56" s="29"/>
+      <c r="T56" s="29"/>
+      <c r="U56" s="29"/>
       <c r="V56" s="21"/>
       <c r="W56" s="21"/>
       <c r="X56" s="21"/>
@@ -5714,16 +5774,18 @@
       <c r="M57" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="N57" s="2"/>
+      <c r="N57" s="2">
+        <v>12</v>
+      </c>
       <c r="O57" s="14" t="str">
         <f t="shared" si="3"/>
-        <v>00</v>
-      </c>
-      <c r="Q57" s="28"/>
-      <c r="R57" s="28"/>
-      <c r="S57" s="28"/>
-      <c r="T57" s="28"/>
-      <c r="U57" s="28"/>
+        <v>0C</v>
+      </c>
+      <c r="Q57" s="29"/>
+      <c r="R57" s="29"/>
+      <c r="S57" s="29"/>
+      <c r="T57" s="29"/>
+      <c r="U57" s="29"/>
       <c r="AG57" s="4"/>
       <c r="AH57" s="4"/>
       <c r="AI57" s="4"/>
@@ -5741,11 +5803,11 @@
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
-      <c r="Q58" s="28"/>
-      <c r="R58" s="28"/>
-      <c r="S58" s="28"/>
-      <c r="T58" s="28"/>
-      <c r="U58" s="28"/>
+      <c r="Q58" s="29"/>
+      <c r="R58" s="29"/>
+      <c r="S58" s="29"/>
+      <c r="T58" s="29"/>
+      <c r="U58" s="29"/>
       <c r="AH58" s="4"/>
       <c r="AI58" s="4"/>
       <c r="AJ58" s="4"/>
@@ -5776,13 +5838,13 @@
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
-      <c r="Q60" s="29" t="s">
+      <c r="Q60" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="R60" s="30"/>
-      <c r="S60" s="30"/>
-      <c r="T60" s="30"/>
-      <c r="U60" s="30"/>
+      <c r="R60" s="31"/>
+      <c r="S60" s="31"/>
+      <c r="T60" s="31"/>
+      <c r="U60" s="31"/>
     </row>
     <row r="61" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L61" s="17" t="s">
@@ -5796,11 +5858,11 @@
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
-      <c r="Q61" s="30"/>
-      <c r="R61" s="30"/>
-      <c r="S61" s="30"/>
-      <c r="T61" s="30"/>
-      <c r="U61" s="30"/>
+      <c r="Q61" s="31"/>
+      <c r="R61" s="31"/>
+      <c r="S61" s="31"/>
+      <c r="T61" s="31"/>
+      <c r="U61" s="31"/>
     </row>
     <row r="62" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L62" s="17" t="s">
@@ -5814,11 +5876,11 @@
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
-      <c r="Q62" s="30"/>
-      <c r="R62" s="30"/>
-      <c r="S62" s="30"/>
-      <c r="T62" s="30"/>
-      <c r="U62" s="30"/>
+      <c r="Q62" s="31"/>
+      <c r="R62" s="31"/>
+      <c r="S62" s="31"/>
+      <c r="T62" s="31"/>
+      <c r="U62" s="31"/>
     </row>
     <row r="63" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L63" s="17" t="s">
@@ -5832,11 +5894,11 @@
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
-      <c r="Q63" s="30"/>
-      <c r="R63" s="30"/>
-      <c r="S63" s="30"/>
-      <c r="T63" s="30"/>
-      <c r="U63" s="30"/>
+      <c r="Q63" s="31"/>
+      <c r="R63" s="31"/>
+      <c r="S63" s="31"/>
+      <c r="T63" s="31"/>
+      <c r="U63" s="31"/>
     </row>
     <row r="64" spans="1:39" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L64" s="17" t="s">
@@ -5850,26 +5912,26 @@
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
-      <c r="Q64" s="30"/>
-      <c r="R64" s="30"/>
-      <c r="S64" s="30"/>
-      <c r="T64" s="30"/>
-      <c r="U64" s="30"/>
-    </row>
-    <row r="65" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q64" s="31"/>
+      <c r="R64" s="31"/>
+      <c r="S64" s="31"/>
+      <c r="T64" s="31"/>
+      <c r="U64" s="31"/>
+    </row>
+    <row r="65" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L65" s="17"/>
       <c r="M65" s="18"/>
       <c r="O65" s="14" t="str">
         <f t="shared" si="3"/>
         <v>00</v>
       </c>
-      <c r="Q65" s="30"/>
-      <c r="R65" s="30"/>
-      <c r="S65" s="30"/>
-      <c r="T65" s="30"/>
-      <c r="U65" s="30"/>
-    </row>
-    <row r="66" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q65" s="31"/>
+      <c r="R65" s="31"/>
+      <c r="S65" s="31"/>
+      <c r="T65" s="31"/>
+      <c r="U65" s="31"/>
+    </row>
+    <row r="66" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L66" s="17"/>
       <c r="M66" s="18"/>
       <c r="O66" s="14" t="str">
@@ -5877,7 +5939,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="67" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L67" s="17"/>
       <c r="M67" s="18"/>
       <c r="O67" s="14" t="str">
@@ -5885,7 +5947,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="68" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L68" s="17"/>
       <c r="M68" s="18"/>
       <c r="O68" s="14" t="str">
@@ -5893,7 +5955,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="69" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L69" s="17"/>
       <c r="M69" s="18"/>
       <c r="O69" s="14" t="str">
@@ -5901,7 +5963,7 @@
         <v>00</v>
       </c>
     </row>
-    <row r="70" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L70" s="17"/>
       <c r="M70" s="18"/>
       <c r="O70" s="14" t="str">
@@ -5909,48 +5971,68 @@
         <v>00</v>
       </c>
     </row>
-    <row r="71" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L71" s="17"/>
       <c r="O71" s="24"/>
     </row>
-    <row r="72" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L72" s="31" t="s">
+    <row r="72" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L72" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="M72" s="32"/>
-      <c r="N72" s="32"/>
-      <c r="O72" s="33"/>
+      <c r="M72" s="33"/>
+      <c r="N72" s="33"/>
+      <c r="O72" s="34"/>
       <c r="AO72" s="4"/>
     </row>
-    <row r="73" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="L73" s="34"/>
-      <c r="M73" s="35"/>
-      <c r="N73" s="35"/>
-      <c r="O73" s="36"/>
-    </row>
-    <row r="74" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="75" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="76" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="77" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="78" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="79" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="80" spans="12:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="81" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="82" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="83" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="84" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="85" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="86" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="87" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="88" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="89" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="90" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="91" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="92" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="93" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="94" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="95" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="96" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="73" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="L73" s="35"/>
+      <c r="M73" s="36"/>
+      <c r="N73" s="36"/>
+      <c r="O73" s="37"/>
+    </row>
+    <row r="74" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="75" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="76" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="77" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="78" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="79" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="80" spans="2:41" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B80" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B81" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B82" s="48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B83" s="25">
+        <v>6700008</v>
+      </c>
+    </row>
+    <row r="84" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="85" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="86" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="87" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="88" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="89" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="90" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="91" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O91" s="25">
+        <v>6700008</v>
+      </c>
+    </row>
+    <row r="92" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="93" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="94" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="95" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="96" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="97" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="98" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="99" ht="14.25" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>